<commit_message>
added cluster summary excel
</commit_message>
<xml_diff>
--- a/scripts/doe_results.xlsx
+++ b/scripts/doe_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chris/cse6242/cse6242-project/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52633499-C060-D24D-8A60-441C31DC5848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A9C575-5169-3A49-B8E2-C76A00A8002C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="5040" windowWidth="28800" windowHeight="16840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3256,7 +3256,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F1FFDB30-F35C-4DE3-8317-D8A5BF5DFE6B}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F1FFDB30-F35C-4DE3-8317-D8A5BF5DFE6B}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:C10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="45">
     <pivotField showAll="0"/>
@@ -3802,7 +3802,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AY55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>

</xml_diff>